<commit_message>
Minor improvements to Prefetch Manager /cache(still not the solid redesign needed)
</commit_message>
<xml_diff>
--- a/PerformanceAnalysis.xlsx
+++ b/PerformanceAnalysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>PDF Physical Render - Optimal</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>(but has memory cost)</t>
+  </si>
+  <si>
+    <t>&gt;&gt;Baseline read, no analysis: Bad Scan Tilted Facing Pages Big -</t>
+  </si>
+  <si>
+    <t>Advantage with single-image render optimization (no analysis)</t>
+  </si>
+  <si>
+    <t>Disadvantage over simple read</t>
+  </si>
+  <si>
+    <t>Middle-of-book performance (start at page 10 instead of 1)</t>
+  </si>
+  <si>
+    <t>Analysis duration Including optimization (and 2nd page invert)</t>
   </si>
 </sst>
 </file>
@@ -134,9 +149,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +162,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,16 +201,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G44"/>
+  <dimension ref="B2:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="B32" sqref="B32:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,11 +552,11 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
-        <f>D10/D4</f>
+        <f t="shared" ref="B4:C8" si="0">D10/D4</f>
         <v>2.6010230179028131</v>
       </c>
       <c r="C4" s="4">
-        <f>E10/E4</f>
+        <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
       <c r="D4" s="1">
@@ -548,11 +574,11 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <f>D11/D5</f>
+        <f t="shared" si="0"/>
         <v>0.97979797979797978</v>
       </c>
       <c r="C5" s="3">
-        <f>E11/E5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D5">
@@ -570,11 +596,11 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <f>D12/D6</f>
+        <f t="shared" si="0"/>
         <v>0.93771626297577859</v>
       </c>
       <c r="C6" s="3">
-        <f>E12/E6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D6">
@@ -592,11 +618,11 @@
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <f>D13/D7</f>
+        <f t="shared" si="0"/>
         <v>1.0073529411764706</v>
       </c>
       <c r="C7" s="3">
-        <f>E13/E7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D7">
@@ -614,11 +640,11 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <f>D14/D8</f>
+        <f t="shared" si="0"/>
         <v>1.6007905138339922</v>
       </c>
       <c r="C8" s="3">
-        <f>E14/E8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D8">
@@ -721,11 +747,11 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
-        <f>D16/D4</f>
+        <f t="shared" ref="B16:C20" si="1">D16/D4</f>
         <v>2.3964194373401533</v>
       </c>
       <c r="C16" s="5">
-        <f>E16/E4</f>
+        <f t="shared" si="1"/>
         <v>3.799145299145299</v>
       </c>
       <c r="D16">
@@ -743,11 +769,11 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
-        <f>D17/D5</f>
+        <f t="shared" si="1"/>
         <v>3.9595959595959598</v>
       </c>
       <c r="C17" s="5">
-        <f>E17/E5</f>
+        <f t="shared" si="1"/>
         <v>3.9356435643564356</v>
       </c>
       <c r="D17">
@@ -765,11 +791,11 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
-        <f>D18/D6</f>
+        <f t="shared" si="1"/>
         <v>3.6505190311418687</v>
       </c>
       <c r="C18" s="5">
-        <f>E18/E6</f>
+        <f t="shared" si="1"/>
         <v>3.1621621621621623</v>
       </c>
       <c r="D18">
@@ -787,11 +813,11 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
-        <f>D19/D7</f>
+        <f t="shared" si="1"/>
         <v>4.2647058823529411</v>
       </c>
       <c r="C19" s="5">
-        <f>E19/E7</f>
+        <f t="shared" si="1"/>
         <v>3.5961538461538463</v>
       </c>
       <c r="D19">
@@ -809,11 +835,11 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
-        <f>D20/D8</f>
+        <f t="shared" si="1"/>
         <v>3.3122529644268774</v>
       </c>
       <c r="C20" s="5">
-        <f>E20/E8</f>
+        <f t="shared" si="1"/>
         <v>4.0148514851485144</v>
       </c>
       <c r="D20">
@@ -830,430 +856,930 @@
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <f>D23-D39</f>
+        <v>624</v>
+      </c>
+      <c r="C23" s="5">
+        <f>E23-E39</f>
+        <v>687</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1057</v>
+      </c>
+      <c r="E23">
+        <v>967</v>
+      </c>
+      <c r="F23">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <f>D24-D40</f>
+        <v>1194</v>
+      </c>
+      <c r="C24" s="5">
+        <f>E24-E40</f>
+        <v>1232</v>
+      </c>
+      <c r="D24" s="5">
+        <v>1471</v>
+      </c>
+      <c r="E24">
+        <v>1497</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <f>D25-D41</f>
+        <v>794</v>
+      </c>
+      <c r="C25" s="5">
+        <f>E25-E41</f>
+        <v>827</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1148</v>
+      </c>
+      <c r="E25">
+        <v>1170</v>
+      </c>
+      <c r="F25">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <f>D26-D42</f>
+        <v>792</v>
+      </c>
+      <c r="C26" s="5">
+        <f>E26-E42</f>
+        <v>765</v>
+      </c>
+      <c r="D26" s="5">
+        <v>977</v>
+      </c>
+      <c r="E26">
+        <v>967</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
+        <f>D27-D43</f>
+        <v>835</v>
+      </c>
+      <c r="C27" s="5">
+        <f>E27-E43</f>
+        <v>842</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1147</v>
+      </c>
+      <c r="E27">
+        <v>1107</v>
+      </c>
+      <c r="F27">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
-        <f>D16-D22</f>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <f>D16-D32</f>
         <v>260</v>
       </c>
-      <c r="C22" s="6">
-        <f>E16-E22</f>
+      <c r="C32" s="6">
+        <f>E16-E32</f>
         <v>375</v>
       </c>
-      <c r="D22">
+      <c r="D32">
         <v>677</v>
       </c>
-      <c r="E22">
+      <c r="E32">
         <v>514</v>
       </c>
-      <c r="F22">
-        <v>15</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F32">
+        <v>15</v>
+      </c>
+      <c r="G32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
-        <f>D17-D23</f>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <f>D17-D33</f>
         <v>425</v>
       </c>
-      <c r="C23" s="6">
-        <f>E17-E23</f>
+      <c r="C33" s="6">
+        <f>E17-E33</f>
         <v>437</v>
       </c>
-      <c r="D23">
+      <c r="D33">
         <v>359</v>
       </c>
-      <c r="E23">
+      <c r="E33">
         <v>358</v>
       </c>
-      <c r="F23">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F33">
+        <v>15</v>
+      </c>
+      <c r="G33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
-        <f>D18-D24</f>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="6">
+        <f>D18-D34</f>
         <v>417</v>
       </c>
-      <c r="C24" s="6">
-        <f>E18-E24</f>
+      <c r="C34" s="6">
+        <f>E18-E34</f>
         <v>297</v>
       </c>
-      <c r="D24">
+      <c r="D34">
         <v>638</v>
       </c>
-      <c r="E24">
+      <c r="E34">
         <v>639</v>
       </c>
-      <c r="F24">
-        <v>15</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F34">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
-        <f>D19-D25</f>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <f>D19-D35</f>
         <v>300</v>
       </c>
-      <c r="C25" s="6">
-        <f>E19-E25</f>
+      <c r="C35" s="6">
+        <f>E19-E35</f>
         <v>265</v>
       </c>
-      <c r="D25">
+      <c r="D35">
         <v>280</v>
       </c>
-      <c r="E25">
+      <c r="E35">
         <v>296</v>
       </c>
-      <c r="F25">
-        <v>15</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F35">
+        <v>15</v>
+      </c>
+      <c r="G35" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
-        <f>D20-D26</f>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <f>D20-D36</f>
         <v>349</v>
       </c>
-      <c r="C26" s="6">
-        <f>E20-E26</f>
+      <c r="C36" s="6">
+        <f>E20-E36</f>
         <v>437</v>
       </c>
-      <c r="D26">
+      <c r="D36">
         <v>489</v>
       </c>
-      <c r="E26">
+      <c r="E36">
         <v>374</v>
       </c>
-      <c r="F26">
+      <c r="F36">
         <v>60</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="37" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="7"/>
+    </row>
+    <row r="39" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="10">
+        <f>D32/D39</f>
+        <v>1.5635103926096998</v>
+      </c>
+      <c r="C39" s="10">
+        <f>E32/E39</f>
+        <v>1.8357142857142856</v>
+      </c>
+      <c r="D39" s="9">
+        <v>433</v>
+      </c>
+      <c r="E39" s="9">
+        <v>280</v>
+      </c>
+      <c r="F39" s="9">
+        <v>15</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="10">
+        <f>D33/D40</f>
+        <v>1.296028880866426</v>
+      </c>
+      <c r="C40" s="10">
+        <f>E33/E40</f>
+        <v>1.350943396226415</v>
+      </c>
+      <c r="D40" s="9">
+        <v>277</v>
+      </c>
+      <c r="E40" s="9">
+        <v>265</v>
+      </c>
+      <c r="F40" s="9">
+        <v>15</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="10">
+        <f>D34/D41</f>
+        <v>1.8022598870056497</v>
+      </c>
+      <c r="C41" s="10">
+        <f>E34/E41</f>
+        <v>1.8629737609329446</v>
+      </c>
+      <c r="D41" s="9">
+        <v>354</v>
+      </c>
+      <c r="E41" s="9">
+        <v>343</v>
+      </c>
+      <c r="F41" s="9">
+        <v>15</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="10">
+        <f>D35/D42</f>
+        <v>1.5135135135135136</v>
+      </c>
+      <c r="C42" s="10">
+        <f>E35/E42</f>
+        <v>1.4653465346534653</v>
+      </c>
+      <c r="D42" s="9">
+        <v>185</v>
+      </c>
+      <c r="E42" s="9">
+        <v>202</v>
+      </c>
+      <c r="F42" s="9">
+        <v>15</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="10">
+        <f>D36/D43</f>
+        <v>1.5673076923076923</v>
+      </c>
+      <c r="C43" s="10">
+        <f>E36/E43</f>
+        <v>1.411320754716981</v>
+      </c>
+      <c r="D43" s="9">
+        <v>312</v>
+      </c>
+      <c r="E43" s="9">
+        <v>265</v>
+      </c>
+      <c r="F43" s="9">
+        <v>60</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="10"/>
+    </row>
+    <row r="46" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="10">
+        <f>D4/D46</f>
+        <v>0.90300230946882221</v>
+      </c>
+      <c r="C46" s="10">
+        <f>E4/E46</f>
+        <v>0.83571428571428574</v>
+      </c>
+      <c r="D46" s="12">
+        <v>433</v>
+      </c>
+      <c r="E46" s="12">
+        <v>280</v>
+      </c>
+      <c r="F46" s="12">
+        <v>15</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="10">
+        <f>D5/D47</f>
+        <v>0.71480144404332135</v>
+      </c>
+      <c r="C47" s="10">
+        <f>E5/E47</f>
+        <v>0.76226415094339628</v>
+      </c>
+      <c r="D47" s="12">
+        <v>277</v>
+      </c>
+      <c r="E47" s="12">
+        <v>265</v>
+      </c>
+      <c r="F47" s="12">
+        <v>15</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="10">
+        <f>D6/D48</f>
+        <v>0.81638418079096042</v>
+      </c>
+      <c r="C48" s="10">
+        <f>E6/E48</f>
+        <v>0.86297376093294464</v>
+      </c>
+      <c r="D48" s="12">
+        <v>354</v>
+      </c>
+      <c r="E48" s="12">
+        <v>343</v>
+      </c>
+      <c r="F48" s="12">
+        <v>15</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="10">
+        <f>D7/D49</f>
+        <v>0.73513513513513518</v>
+      </c>
+      <c r="C49" s="10">
+        <f>E7/E49</f>
+        <v>0.7722772277227723</v>
+      </c>
+      <c r="D49" s="12">
+        <v>185</v>
+      </c>
+      <c r="E49" s="12">
+        <v>202</v>
+      </c>
+      <c r="F49" s="12">
+        <v>15</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="10">
+        <f>D8/D50</f>
+        <v>0.8108974358974359</v>
+      </c>
+      <c r="C50" s="10">
+        <f>E8/E50</f>
+        <v>0.76226415094339628</v>
+      </c>
+      <c r="D50" s="12">
+        <v>312</v>
+      </c>
+      <c r="E50" s="12">
+        <v>265</v>
+      </c>
+      <c r="F50" s="12">
+        <v>60</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="52" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="10">
+        <f>D39/D53</f>
+        <v>0.94748358862144422</v>
+      </c>
+      <c r="C53" s="10">
+        <f>E39/E53</f>
+        <v>1</v>
+      </c>
+      <c r="D53" s="9">
+        <v>457</v>
+      </c>
+      <c r="E53" s="9">
+        <v>280</v>
+      </c>
+      <c r="F53" s="9">
+        <v>15</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="10">
+        <f>D40/D54</f>
+        <v>1.0613026819923372</v>
+      </c>
+      <c r="C54" s="10">
+        <f>E40/E54</f>
+        <v>1</v>
+      </c>
+      <c r="D54" s="9">
+        <v>261</v>
+      </c>
+      <c r="E54" s="9">
+        <v>265</v>
+      </c>
+      <c r="F54" s="9">
+        <v>12</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="10">
+        <f>D41/D55</f>
+        <v>0.95675675675675675</v>
+      </c>
+      <c r="C55" s="10">
+        <f>E41/E55</f>
+        <v>0.95810055865921784</v>
+      </c>
+      <c r="D55" s="9">
+        <v>370</v>
+      </c>
+      <c r="E55" s="9">
+        <v>358</v>
+      </c>
+      <c r="F55" s="9">
+        <v>15</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="10">
+        <f>D42/D56</f>
+        <v>0.86854460093896713</v>
+      </c>
+      <c r="C56" s="10">
+        <f>E42/E56</f>
+        <v>0.92660550458715596</v>
+      </c>
+      <c r="D56" s="9">
+        <v>213</v>
+      </c>
+      <c r="E56" s="9">
+        <v>218</v>
+      </c>
+      <c r="F56" s="9">
+        <v>15</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="10">
+        <f>D43/D57</f>
+        <v>0.95121951219512191</v>
+      </c>
+      <c r="C57" s="10">
+        <f>E43/E57</f>
+        <v>0.9464285714285714</v>
+      </c>
+      <c r="D57" s="9">
+        <v>328</v>
+      </c>
+      <c r="E57" s="9">
+        <v>280</v>
+      </c>
+      <c r="F57" s="9">
+        <v>57</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="2:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
-        <f>D16/D28</f>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="7">
+        <f>D16/D61</f>
         <v>49.315789473684212</v>
       </c>
-      <c r="C28" s="7">
-        <f>E16/E28</f>
+      <c r="C61" s="7">
+        <f>E16/E61</f>
         <v>59.266666666666666</v>
       </c>
-      <c r="D28">
+      <c r="D61">
         <v>19</v>
       </c>
-      <c r="E28">
-        <v>15</v>
-      </c>
-      <c r="F28">
-        <v>15</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="E61">
+        <v>15</v>
+      </c>
+      <c r="F61">
+        <v>15</v>
+      </c>
+      <c r="G61" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="7">
-        <f>D17/D29</f>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="7">
+        <f>D17/D62</f>
         <v>8.615384615384615</v>
       </c>
-      <c r="C29" s="7">
-        <f>E17/E29</f>
+      <c r="C62" s="7">
+        <f>E17/E62</f>
         <v>8.5483870967741939</v>
       </c>
-      <c r="D29">
+      <c r="D62">
         <v>91</v>
       </c>
-      <c r="E29">
+      <c r="E62">
         <v>93</v>
       </c>
-      <c r="F29">
-        <v>15</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="F62">
+        <v>15</v>
+      </c>
+      <c r="G62" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="7">
-        <f>D18/D30</f>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="7">
+        <f>D18/D63</f>
         <v>12.55952380952381</v>
       </c>
-      <c r="C30" s="7">
-        <f>E18/E30</f>
+      <c r="C63" s="7">
+        <f>E18/E63</f>
         <v>20.347826086956523</v>
       </c>
-      <c r="D30">
+      <c r="D63">
         <v>84</v>
       </c>
-      <c r="E30">
+      <c r="E63">
         <v>46</v>
       </c>
-      <c r="F30">
-        <v>15</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F63">
+        <v>15</v>
+      </c>
+      <c r="G63" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="7">
-        <f>D19/D31</f>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="7">
+        <f>D19/D64</f>
         <v>7.6315789473684212</v>
       </c>
-      <c r="C31" s="7">
-        <f>E19/E31</f>
+      <c r="C64" s="7">
+        <f>E19/E64</f>
         <v>9.0483870967741939</v>
       </c>
-      <c r="D31">
+      <c r="D64">
         <v>76</v>
       </c>
-      <c r="E31">
+      <c r="E64">
         <v>62</v>
       </c>
-      <c r="F31">
-        <v>15</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F64">
+        <v>15</v>
+      </c>
+      <c r="G64" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="7">
-        <f>D20/D32</f>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="7">
+        <f>D20/D65</f>
         <v>12.323529411764707</v>
       </c>
-      <c r="C32" s="7">
-        <f>E20/E32</f>
+      <c r="C65" s="7">
+        <f>E20/E65</f>
         <v>13.080645161290322</v>
       </c>
-      <c r="D32">
+      <c r="D65">
         <v>68</v>
       </c>
-      <c r="E32">
+      <c r="E65">
         <v>62</v>
       </c>
-      <c r="F32">
+      <c r="F65">
         <v>60</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G65" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="7">
-        <f>D4/D34</f>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="7">
+        <f>D4/D67</f>
         <v>20.578947368421051</v>
       </c>
-      <c r="C34" s="7">
-        <f>E4/E34</f>
+      <c r="C67" s="7">
+        <f>E4/E67</f>
         <v>15.6</v>
       </c>
-      <c r="D34">
+      <c r="D67" s="11">
         <v>19</v>
       </c>
-      <c r="E34">
-        <v>15</v>
-      </c>
-      <c r="F34">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="E67" s="11">
+        <v>15</v>
+      </c>
+      <c r="F67" s="11">
+        <v>15</v>
+      </c>
+      <c r="G67" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="7">
-        <f>D5/D35</f>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="7">
+        <f>D5/D68</f>
         <v>2.1758241758241756</v>
       </c>
-      <c r="C35" s="7">
-        <f>E5/E35</f>
+      <c r="C68" s="7">
+        <f>E5/E68</f>
         <v>2.172043010752688</v>
       </c>
-      <c r="D35">
+      <c r="D68" s="11">
         <v>91</v>
       </c>
-      <c r="E35">
+      <c r="E68" s="11">
         <v>93</v>
       </c>
-      <c r="F35">
-        <v>15</v>
-      </c>
-      <c r="G35" t="s">
+      <c r="F68" s="11">
+        <v>15</v>
+      </c>
+      <c r="G68" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="7">
-        <f>D6/D36</f>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="7">
+        <f>D6/D69</f>
         <v>3.4404761904761907</v>
       </c>
-      <c r="C36" s="7">
-        <f>E6/E36</f>
+      <c r="C69" s="7">
+        <f>E6/E69</f>
         <v>6.4347826086956523</v>
       </c>
-      <c r="D36">
+      <c r="D69" s="11">
         <v>84</v>
       </c>
-      <c r="E36">
+      <c r="E69" s="11">
         <v>46</v>
       </c>
-      <c r="F36">
-        <v>15</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="F69" s="11">
+        <v>15</v>
+      </c>
+      <c r="G69" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
-        <f>D7/D37</f>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="7">
+        <f>D7/D70</f>
         <v>1.7894736842105263</v>
       </c>
-      <c r="C37" s="7">
-        <f>E7/E37</f>
+      <c r="C70" s="7">
+        <f>E7/E70</f>
         <v>2.5161290322580645</v>
       </c>
-      <c r="D37">
+      <c r="D70" s="11">
         <v>76</v>
       </c>
-      <c r="E37">
+      <c r="E70" s="11">
         <v>62</v>
       </c>
-      <c r="F37">
-        <v>15</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F70" s="11">
+        <v>15</v>
+      </c>
+      <c r="G70" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
-        <f>D8/D38</f>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="7">
+        <f>D8/D71</f>
         <v>3.7205882352941178</v>
       </c>
-      <c r="C38" s="7">
-        <f>E8/E38</f>
+      <c r="C71" s="7">
+        <f>E8/E71</f>
         <v>3.2580645161290325</v>
       </c>
-      <c r="D38">
+      <c r="D71" s="11">
         <v>68</v>
       </c>
-      <c r="E38">
+      <c r="E71" s="11">
         <v>62</v>
       </c>
-      <c r="F38">
+      <c r="F71" s="11">
         <v>60</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G71" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40">
+      <c r="C73" s="8"/>
+      <c r="D73">
         <v>5</v>
       </c>
-      <c r="E40">
+      <c r="E73">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>15</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="F73">
+        <v>15</v>
+      </c>
+      <c r="G73" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>36</v>
       </c>
-      <c r="D41">
+      <c r="D74">
         <v>2</v>
       </c>
-      <c r="E41">
+      <c r="E74">
         <v>0</v>
       </c>
-      <c r="F41">
-        <v>15</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="F74">
+        <v>15</v>
+      </c>
+      <c r="G74" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D42">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D75">
         <v>6</v>
       </c>
-      <c r="E42">
+      <c r="E75">
         <v>0</v>
       </c>
-      <c r="F42">
-        <v>15</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="F75">
+        <v>15</v>
+      </c>
+      <c r="G75" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D43">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D76">
         <v>6</v>
       </c>
-      <c r="E43">
+      <c r="E76">
         <v>0</v>
       </c>
-      <c r="F43">
-        <v>15</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="F76">
+        <v>15</v>
+      </c>
+      <c r="G76" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D44">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D77">
         <v>1</v>
       </c>
-      <c r="E44">
+      <c r="E77">
         <v>0</v>
       </c>
-      <c r="F44">
+      <c r="F77">
         <v>60</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G77" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:E33 D39:E39 D45:E1048576 D40:D44">
-    <cfRule type="dataBar" priority="3">
+  <conditionalFormatting sqref="D72:E72 D1:E22 D78:E1048576 D73:D77 D59:E66 D39:D45 D28:E38 E23:E27">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1266,8 +1792,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:E38">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="D67:E71">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1280,8 +1806,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:E1048576">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="D59:E1048576 D1:E22 D39:D45 D28:E38 E23:E27">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1294,7 +1820,78 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D46:D52 D58">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BA8A5E4B-47FE-4601-AD2B-A0A238A7EBC7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58:E1048576 D1:E22 E53:E57 D28:E52 E23:E27">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3B3AFA4E-EB13-4CA3-81B6-D648F4F1CEF4}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D57">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{47998C63-E9BE-4A98-944B-85D27FBCD9D2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D57">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{06DD8368-4769-4E9D-8FD6-4DB96CA2E55E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D53:D57">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F7AE4CFA-BB07-4C7E-A3DF-0195F0567E4E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1307,7 +1904,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D1:E33 D39:E39 D45:E1048576 D40:D44</xm:sqref>
+          <xm:sqref>D72:E72 D1:E22 D78:E1048576 D73:D77 D59:E66 D39:D45 D28:E38 E23:E27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4D80F0E5-E95D-42C4-9BAD-97EC4FE675A1}">
@@ -1318,7 +1915,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34:E38</xm:sqref>
+          <xm:sqref>D67:E71</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{30FF35A2-9BE5-4A21-9597-A55976695ADE}">
@@ -1329,7 +1926,62 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D1:E1048576</xm:sqref>
+          <xm:sqref>D59:E1048576 D1:E22 D39:D45 D28:E38 E23:E27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BA8A5E4B-47FE-4601-AD2B-A0A238A7EBC7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D46:D52 D58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3B3AFA4E-EB13-4CA3-81B6-D648F4F1CEF4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D58:E1048576 D1:E22 E53:E57 D28:E52 E23:E27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{47998C63-E9BE-4A98-944B-85D27FBCD9D2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D53:D57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{06DD8368-4769-4E9D-8FD6-4DB96CA2E55E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D53:D57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F7AE4CFA-BB07-4C7E-A3DF-0195F0567E4E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D53:D57</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>